<commit_message>
update Type Of Resource Field Name
</commit_message>
<xml_diff>
--- a/metadata_templates/HP_AV_complex_metadata_template.xlsx
+++ b/metadata_templates/HP_AV_complex_metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelbolam/Documents/GitHub/MAD_Islandora_Metadata/islandora_metadata/metadata_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179F935-1CC2-6745-A862-83468430B883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB7E0DC-CDED-F243-AA89-EF05694E0C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28940" yWindow="-6880" windowWidth="29280" windowHeight="19360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32360" yWindow="-6780" windowWidth="29280" windowHeight="19360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>genre</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>identifier</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>batch</t>
+  </si>
+  <si>
+    <t>type_of_resource</t>
   </si>
 </sst>
 </file>
@@ -622,10 +622,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AEA105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,82 +661,82 @@
   <sheetData>
     <row r="1" spans="1:26" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="R1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1592,16 +1592,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>